<commit_message>
version 6.1, add logs, invalid sessions collector, refactor code, and so one
</commit_message>
<xml_diff>
--- a/res/gmail.xlsx
+++ b/res/gmail.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,153 +453,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>meghanhines756@gmail.com</t>
+          <t>olganovikov53583@gmail.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>wAv!ecig%o39%10</t>
+          <t>koh93hwlz3ilw7</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8yaxjuliaroberts2@web.de</t>
+          <t>7knkeepdontity1999zu@aol.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>minglis147@gmail.com</t>
+          <t>rozaskiara882@gmail.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Zyge!mozu%t5ys&amp;o</t>
+          <t>gwpgp6nd6qmkc</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>zoanarasius199432@mail.ru</t>
+          <t>tdcounandarse2011c5@yahoo.ca</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>mldrdsinclair@gmail.com</t>
+          <t>thidphymee@gmail.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6860bYso%c#ih$AXY</t>
+          <t>n0z3ba7rgn6vfo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25maetasporton44@sharklasers.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>pomidorka2m6@gmail.com</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>$PYz!oLiMeqowIMi9s</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2rpomidorka2h50a0@10mail.org</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>pops991n@gmail.com</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Ri!qew!u5k</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>oopops9919@guerrillamail.org</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>rendjasper841@gmail.com</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>#S&amp;4418OVIf</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>herendjasper841@telus.net</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>smailik582n@gmail.com</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>legEBo##H&amp;39</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>xismailik58265@mailexpire.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>spear2002n@gmail.com</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CuHuD323OD!i&amp;lE</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>rjspear2002@ymail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>stepastepancherry3@gmail.com</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>h$Ucoci$!39L</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>jmstepastepancherry36@guerrillamail.com</t>
+          <t>pv2roychrisicke@divermail.com</t>
         </is>
       </c>
     </row>

</xml_diff>